<commit_message>
added Load Balancing to backend
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan Tourify.xlsx
+++ b/documentation/Zeitplan Tourify.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA58F59-7F5D-4DD8-888A-7D83B3081048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF7EBE-2D7F-4B05-A34D-700F6950E353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="950" yWindow="0" windowWidth="18250" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Task 3</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Routen erstellen</t>
+  </si>
+  <si>
+    <t>Load Balancing</t>
   </si>
 </sst>
 </file>
@@ -289,7 +292,7 @@
     <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="d"/>
-    <numFmt numFmtId="172" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="169" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -921,71 +924,71 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="9" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="9" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="9" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="9" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1553,11 +1556,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL33"/>
+  <dimension ref="A1:BL34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1600,107 +1603,107 @@
         <v>37</v>
       </c>
       <c r="B3" s="57"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="80">
+      <c r="D3" s="96"/>
+      <c r="E3" s="94">
         <f>DATE(2022,3,21)</f>
         <v>44641</v>
       </c>
-      <c r="F3" s="80"/>
+      <c r="F3" s="94"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="91">
         <f>I5</f>
         <v>44641</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="77">
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="91">
         <f>P5</f>
         <v>44648</v>
       </c>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="77">
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="91">
         <f>W5</f>
         <v>44655</v>
       </c>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="77">
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="91">
         <f>AD5</f>
         <v>44662</v>
       </c>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="78"/>
-      <c r="AG4" s="78"/>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="77">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="91">
         <f>AK5</f>
         <v>44669</v>
       </c>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="78"/>
-      <c r="AN4" s="78"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="77">
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="91">
         <f>AR5</f>
         <v>44676</v>
       </c>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="78"/>
-      <c r="AU4" s="78"/>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="77">
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="91">
         <f>AY5</f>
         <v>44683</v>
       </c>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="78"/>
-      <c r="BB4" s="78"/>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="77">
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="91">
         <f>BF5</f>
         <v>44690</v>
       </c>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="78"/>
-      <c r="BI4" s="78"/>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="79"/>
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="93"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="52" t="s">
@@ -2265,7 +2268,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H29" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H30" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="38"/>
@@ -2338,11 +2341,11 @@
       <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="77">
         <f>Project_Start</f>
         <v>44641</v>
       </c>
-      <c r="F9" s="83">
+      <c r="F9" s="77">
         <f>E9+0</f>
         <v>44641</v>
       </c>
@@ -2352,44 +2355,44 @@
         <v>1</v>
       </c>
       <c r="I9" s="38"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="81"/>
-      <c r="Z9" s="81"/>
-      <c r="AA9" s="81"/>
-      <c r="AB9" s="81"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="81"/>
-      <c r="AE9" s="81"/>
-      <c r="AF9" s="81"/>
-      <c r="AG9" s="81"/>
-      <c r="AH9" s="81"/>
-      <c r="AI9" s="81"/>
-      <c r="AJ9" s="81"/>
-      <c r="AK9" s="81"/>
-      <c r="AL9" s="81"/>
-      <c r="AM9" s="81"/>
-      <c r="AN9" s="81"/>
-      <c r="AO9" s="81"/>
-      <c r="AP9" s="81"/>
-      <c r="AQ9" s="81"/>
-      <c r="AR9" s="81"/>
-      <c r="AS9" s="81"/>
-      <c r="AT9" s="81"/>
-      <c r="AU9" s="81"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="75"/>
+      <c r="AB9" s="75"/>
+      <c r="AC9" s="75"/>
+      <c r="AD9" s="75"/>
+      <c r="AE9" s="75"/>
+      <c r="AF9" s="75"/>
+      <c r="AG9" s="75"/>
+      <c r="AH9" s="75"/>
+      <c r="AI9" s="75"/>
+      <c r="AJ9" s="75"/>
+      <c r="AK9" s="75"/>
+      <c r="AL9" s="75"/>
+      <c r="AM9" s="75"/>
+      <c r="AN9" s="75"/>
+      <c r="AO9" s="75"/>
+      <c r="AP9" s="75"/>
+      <c r="AQ9" s="75"/>
+      <c r="AR9" s="75"/>
+      <c r="AS9" s="75"/>
+      <c r="AT9" s="75"/>
+      <c r="AU9" s="75"/>
       <c r="AV9" s="38"/>
       <c r="AW9" s="38"/>
       <c r="AX9" s="38"/>
@@ -2421,11 +2424,11 @@
       <c r="D10" s="22">
         <v>1</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="77">
         <f>F9</f>
         <v>44641</v>
       </c>
-      <c r="F10" s="83">
+      <c r="F10" s="77">
         <f>E10+0</f>
         <v>44641</v>
       </c>
@@ -2435,44 +2438,44 @@
         <v>1</v>
       </c>
       <c r="I10" s="38"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="82"/>
-      <c r="V10" s="82"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="81"/>
-      <c r="AD10" s="81"/>
-      <c r="AE10" s="81"/>
-      <c r="AF10" s="81"/>
-      <c r="AG10" s="81"/>
-      <c r="AH10" s="81"/>
-      <c r="AI10" s="81"/>
-      <c r="AJ10" s="81"/>
-      <c r="AK10" s="81"/>
-      <c r="AL10" s="81"/>
-      <c r="AM10" s="81"/>
-      <c r="AN10" s="81"/>
-      <c r="AO10" s="81"/>
-      <c r="AP10" s="81"/>
-      <c r="AQ10" s="81"/>
-      <c r="AR10" s="81"/>
-      <c r="AS10" s="81"/>
-      <c r="AT10" s="81"/>
-      <c r="AU10" s="81"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+      <c r="T10" s="75"/>
+      <c r="U10" s="76"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="75"/>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="75"/>
+      <c r="AA10" s="75"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="75"/>
+      <c r="AD10" s="75"/>
+      <c r="AE10" s="75"/>
+      <c r="AF10" s="75"/>
+      <c r="AG10" s="75"/>
+      <c r="AH10" s="75"/>
+      <c r="AI10" s="75"/>
+      <c r="AJ10" s="75"/>
+      <c r="AK10" s="75"/>
+      <c r="AL10" s="75"/>
+      <c r="AM10" s="75"/>
+      <c r="AN10" s="75"/>
+      <c r="AO10" s="75"/>
+      <c r="AP10" s="75"/>
+      <c r="AQ10" s="75"/>
+      <c r="AR10" s="75"/>
+      <c r="AS10" s="75"/>
+      <c r="AT10" s="75"/>
+      <c r="AU10" s="75"/>
       <c r="AV10" s="38"/>
       <c r="AW10" s="38"/>
       <c r="AX10" s="38"/>
@@ -2502,11 +2505,11 @@
       <c r="D11" s="22">
         <v>1</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="77">
         <f>F10</f>
         <v>44641</v>
       </c>
-      <c r="F11" s="83">
+      <c r="F11" s="77">
         <f>E11+1</f>
         <v>44642</v>
       </c>
@@ -2516,44 +2519,44 @@
         <v>2</v>
       </c>
       <c r="I11" s="38"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="81"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
-      <c r="Y11" s="81"/>
-      <c r="Z11" s="81"/>
-      <c r="AA11" s="81"/>
-      <c r="AB11" s="81"/>
-      <c r="AC11" s="81"/>
-      <c r="AD11" s="81"/>
-      <c r="AE11" s="81"/>
-      <c r="AF11" s="81"/>
-      <c r="AG11" s="81"/>
-      <c r="AH11" s="81"/>
-      <c r="AI11" s="81"/>
-      <c r="AJ11" s="81"/>
-      <c r="AK11" s="81"/>
-      <c r="AL11" s="81"/>
-      <c r="AM11" s="81"/>
-      <c r="AN11" s="81"/>
-      <c r="AO11" s="81"/>
-      <c r="AP11" s="81"/>
-      <c r="AQ11" s="81"/>
-      <c r="AR11" s="81"/>
-      <c r="AS11" s="81"/>
-      <c r="AT11" s="81"/>
-      <c r="AU11" s="81"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="75"/>
+      <c r="V11" s="75"/>
+      <c r="W11" s="75"/>
+      <c r="X11" s="75"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="75"/>
+      <c r="AA11" s="75"/>
+      <c r="AB11" s="75"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="75"/>
+      <c r="AE11" s="75"/>
+      <c r="AF11" s="75"/>
+      <c r="AG11" s="75"/>
+      <c r="AH11" s="75"/>
+      <c r="AI11" s="75"/>
+      <c r="AJ11" s="75"/>
+      <c r="AK11" s="75"/>
+      <c r="AL11" s="75"/>
+      <c r="AM11" s="75"/>
+      <c r="AN11" s="75"/>
+      <c r="AO11" s="75"/>
+      <c r="AP11" s="75"/>
+      <c r="AQ11" s="75"/>
+      <c r="AR11" s="75"/>
+      <c r="AS11" s="75"/>
+      <c r="AT11" s="75"/>
+      <c r="AU11" s="75"/>
       <c r="AV11" s="38"/>
       <c r="AW11" s="38"/>
       <c r="AX11" s="38"/>
@@ -2581,52 +2584,52 @@
       </c>
       <c r="C12" s="61"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I12" s="38"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
-      <c r="S12" s="81"/>
-      <c r="T12" s="81"/>
-      <c r="U12" s="81"/>
-      <c r="V12" s="81"/>
-      <c r="W12" s="81"/>
-      <c r="X12" s="81"/>
-      <c r="Y12" s="81"/>
-      <c r="Z12" s="81"/>
-      <c r="AA12" s="81"/>
-      <c r="AB12" s="81"/>
-      <c r="AC12" s="81"/>
-      <c r="AD12" s="81"/>
-      <c r="AE12" s="81"/>
-      <c r="AF12" s="81"/>
-      <c r="AG12" s="81"/>
-      <c r="AH12" s="81"/>
-      <c r="AI12" s="81"/>
-      <c r="AJ12" s="81"/>
-      <c r="AK12" s="81"/>
-      <c r="AL12" s="81"/>
-      <c r="AM12" s="81"/>
-      <c r="AN12" s="81"/>
-      <c r="AO12" s="81"/>
-      <c r="AP12" s="81"/>
-      <c r="AQ12" s="81"/>
-      <c r="AR12" s="81"/>
-      <c r="AS12" s="81"/>
-      <c r="AT12" s="81"/>
-      <c r="AU12" s="81"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+      <c r="U12" s="75"/>
+      <c r="V12" s="75"/>
+      <c r="W12" s="75"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="75"/>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="75"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="75"/>
+      <c r="AF12" s="75"/>
+      <c r="AG12" s="75"/>
+      <c r="AH12" s="75"/>
+      <c r="AI12" s="75"/>
+      <c r="AJ12" s="75"/>
+      <c r="AK12" s="75"/>
+      <c r="AL12" s="75"/>
+      <c r="AM12" s="75"/>
+      <c r="AN12" s="75"/>
+      <c r="AO12" s="75"/>
+      <c r="AP12" s="75"/>
+      <c r="AQ12" s="75"/>
+      <c r="AR12" s="75"/>
+      <c r="AS12" s="75"/>
+      <c r="AT12" s="75"/>
+      <c r="AU12" s="75"/>
       <c r="AV12" s="38"/>
       <c r="AW12" s="38"/>
       <c r="AX12" s="38"/>
@@ -2656,11 +2659,11 @@
       <c r="D13" s="25">
         <v>1</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="80">
         <f>F11+0</f>
         <v>44642</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="80">
         <f>E13+3</f>
         <v>44645</v>
       </c>
@@ -2670,44 +2673,44 @@
         <v>4</v>
       </c>
       <c r="I13" s="38"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="81"/>
-      <c r="Z13" s="81"/>
-      <c r="AA13" s="81"/>
-      <c r="AB13" s="81"/>
-      <c r="AC13" s="81"/>
-      <c r="AD13" s="81"/>
-      <c r="AE13" s="81"/>
-      <c r="AF13" s="81"/>
-      <c r="AG13" s="81"/>
-      <c r="AH13" s="81"/>
-      <c r="AI13" s="81"/>
-      <c r="AJ13" s="81"/>
-      <c r="AK13" s="81"/>
-      <c r="AL13" s="81"/>
-      <c r="AM13" s="81"/>
-      <c r="AN13" s="81"/>
-      <c r="AO13" s="81"/>
-      <c r="AP13" s="81"/>
-      <c r="AQ13" s="81"/>
-      <c r="AR13" s="81"/>
-      <c r="AS13" s="81"/>
-      <c r="AT13" s="81"/>
-      <c r="AU13" s="81"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="75"/>
+      <c r="V13" s="75"/>
+      <c r="W13" s="75"/>
+      <c r="X13" s="75"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="75"/>
+      <c r="AA13" s="75"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="75"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="75"/>
+      <c r="AG13" s="75"/>
+      <c r="AH13" s="75"/>
+      <c r="AI13" s="75"/>
+      <c r="AJ13" s="75"/>
+      <c r="AK13" s="75"/>
+      <c r="AL13" s="75"/>
+      <c r="AM13" s="75"/>
+      <c r="AN13" s="75"/>
+      <c r="AO13" s="75"/>
+      <c r="AP13" s="75"/>
+      <c r="AQ13" s="75"/>
+      <c r="AR13" s="75"/>
+      <c r="AS13" s="75"/>
+      <c r="AT13" s="75"/>
+      <c r="AU13" s="75"/>
       <c r="AV13" s="38"/>
       <c r="AW13" s="38"/>
       <c r="AX13" s="38"/>
@@ -2737,10 +2740,10 @@
       <c r="D14" s="25">
         <v>1</v>
       </c>
-      <c r="E14" s="86">
+      <c r="E14" s="80">
         <v>44642</v>
       </c>
-      <c r="F14" s="86">
+      <c r="F14" s="80">
         <f>E14+10</f>
         <v>44652</v>
       </c>
@@ -2750,44 +2753,44 @@
         <v>11</v>
       </c>
       <c r="I14" s="38"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="81"/>
-      <c r="S14" s="81"/>
-      <c r="T14" s="81"/>
-      <c r="U14" s="82"/>
-      <c r="V14" s="82"/>
-      <c r="W14" s="81"/>
-      <c r="X14" s="81"/>
-      <c r="Y14" s="81"/>
-      <c r="Z14" s="81"/>
-      <c r="AA14" s="81"/>
-      <c r="AB14" s="81"/>
-      <c r="AC14" s="81"/>
-      <c r="AD14" s="81"/>
-      <c r="AE14" s="81"/>
-      <c r="AF14" s="81"/>
-      <c r="AG14" s="81"/>
-      <c r="AH14" s="81"/>
-      <c r="AI14" s="81"/>
-      <c r="AJ14" s="81"/>
-      <c r="AK14" s="81"/>
-      <c r="AL14" s="81"/>
-      <c r="AM14" s="81"/>
-      <c r="AN14" s="81"/>
-      <c r="AO14" s="81"/>
-      <c r="AP14" s="81"/>
-      <c r="AQ14" s="81"/>
-      <c r="AR14" s="81"/>
-      <c r="AS14" s="81"/>
-      <c r="AT14" s="81"/>
-      <c r="AU14" s="81"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
+      <c r="S14" s="75"/>
+      <c r="T14" s="75"/>
+      <c r="U14" s="76"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="75"/>
+      <c r="X14" s="75"/>
+      <c r="Y14" s="75"/>
+      <c r="Z14" s="75"/>
+      <c r="AA14" s="75"/>
+      <c r="AB14" s="75"/>
+      <c r="AC14" s="75"/>
+      <c r="AD14" s="75"/>
+      <c r="AE14" s="75"/>
+      <c r="AF14" s="75"/>
+      <c r="AG14" s="75"/>
+      <c r="AH14" s="75"/>
+      <c r="AI14" s="75"/>
+      <c r="AJ14" s="75"/>
+      <c r="AK14" s="75"/>
+      <c r="AL14" s="75"/>
+      <c r="AM14" s="75"/>
+      <c r="AN14" s="75"/>
+      <c r="AO14" s="75"/>
+      <c r="AP14" s="75"/>
+      <c r="AQ14" s="75"/>
+      <c r="AR14" s="75"/>
+      <c r="AS14" s="75"/>
+      <c r="AT14" s="75"/>
+      <c r="AU14" s="75"/>
       <c r="AV14" s="38"/>
       <c r="AW14" s="38"/>
       <c r="AX14" s="38"/>
@@ -2817,10 +2820,10 @@
       <c r="D15" s="25">
         <v>1</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="80">
         <v>44642</v>
       </c>
-      <c r="F15" s="86">
+      <c r="F15" s="80">
         <f>E15+3</f>
         <v>44645</v>
       </c>
@@ -2830,44 +2833,44 @@
         <v>4</v>
       </c>
       <c r="I15" s="38"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="81"/>
-      <c r="S15" s="81"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="81"/>
-      <c r="V15" s="81"/>
-      <c r="W15" s="81"/>
-      <c r="X15" s="81"/>
-      <c r="Y15" s="81"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="81"/>
-      <c r="AB15" s="81"/>
-      <c r="AC15" s="81"/>
-      <c r="AD15" s="81"/>
-      <c r="AE15" s="81"/>
-      <c r="AF15" s="81"/>
-      <c r="AG15" s="81"/>
-      <c r="AH15" s="81"/>
-      <c r="AI15" s="81"/>
-      <c r="AJ15" s="81"/>
-      <c r="AK15" s="81"/>
-      <c r="AL15" s="81"/>
-      <c r="AM15" s="81"/>
-      <c r="AN15" s="81"/>
-      <c r="AO15" s="81"/>
-      <c r="AP15" s="81"/>
-      <c r="AQ15" s="81"/>
-      <c r="AR15" s="81"/>
-      <c r="AS15" s="81"/>
-      <c r="AT15" s="81"/>
-      <c r="AU15" s="81"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="75"/>
+      <c r="V15" s="75"/>
+      <c r="W15" s="75"/>
+      <c r="X15" s="75"/>
+      <c r="Y15" s="75"/>
+      <c r="Z15" s="75"/>
+      <c r="AA15" s="75"/>
+      <c r="AB15" s="75"/>
+      <c r="AC15" s="75"/>
+      <c r="AD15" s="75"/>
+      <c r="AE15" s="75"/>
+      <c r="AF15" s="75"/>
+      <c r="AG15" s="75"/>
+      <c r="AH15" s="75"/>
+      <c r="AI15" s="75"/>
+      <c r="AJ15" s="75"/>
+      <c r="AK15" s="75"/>
+      <c r="AL15" s="75"/>
+      <c r="AM15" s="75"/>
+      <c r="AN15" s="75"/>
+      <c r="AO15" s="75"/>
+      <c r="AP15" s="75"/>
+      <c r="AQ15" s="75"/>
+      <c r="AR15" s="75"/>
+      <c r="AS15" s="75"/>
+      <c r="AT15" s="75"/>
+      <c r="AU15" s="75"/>
       <c r="AV15" s="38"/>
       <c r="AW15" s="38"/>
       <c r="AX15" s="38"/>
@@ -2897,11 +2900,11 @@
       <c r="D16" s="25">
         <v>1</v>
       </c>
-      <c r="E16" s="86">
+      <c r="E16" s="80">
         <f>E15</f>
         <v>44642</v>
       </c>
-      <c r="F16" s="86">
+      <c r="F16" s="80">
         <f>E16+3</f>
         <v>44645</v>
       </c>
@@ -2911,44 +2914,44 @@
         <v>4</v>
       </c>
       <c r="I16" s="38"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="81"/>
-      <c r="S16" s="81"/>
-      <c r="T16" s="81"/>
-      <c r="U16" s="81"/>
-      <c r="V16" s="81"/>
-      <c r="W16" s="81"/>
-      <c r="X16" s="81"/>
-      <c r="Y16" s="82"/>
-      <c r="Z16" s="81"/>
-      <c r="AA16" s="81"/>
-      <c r="AB16" s="81"/>
-      <c r="AC16" s="81"/>
-      <c r="AD16" s="81"/>
-      <c r="AE16" s="81"/>
-      <c r="AF16" s="81"/>
-      <c r="AG16" s="81"/>
-      <c r="AH16" s="81"/>
-      <c r="AI16" s="81"/>
-      <c r="AJ16" s="81"/>
-      <c r="AK16" s="81"/>
-      <c r="AL16" s="81"/>
-      <c r="AM16" s="81"/>
-      <c r="AN16" s="81"/>
-      <c r="AO16" s="81"/>
-      <c r="AP16" s="81"/>
-      <c r="AQ16" s="81"/>
-      <c r="AR16" s="81"/>
-      <c r="AS16" s="81"/>
-      <c r="AT16" s="81"/>
-      <c r="AU16" s="81"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="75"/>
+      <c r="U16" s="75"/>
+      <c r="V16" s="75"/>
+      <c r="W16" s="75"/>
+      <c r="X16" s="75"/>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="75"/>
+      <c r="AA16" s="75"/>
+      <c r="AB16" s="75"/>
+      <c r="AC16" s="75"/>
+      <c r="AD16" s="75"/>
+      <c r="AE16" s="75"/>
+      <c r="AF16" s="75"/>
+      <c r="AG16" s="75"/>
+      <c r="AH16" s="75"/>
+      <c r="AI16" s="75"/>
+      <c r="AJ16" s="75"/>
+      <c r="AK16" s="75"/>
+      <c r="AL16" s="75"/>
+      <c r="AM16" s="75"/>
+      <c r="AN16" s="75"/>
+      <c r="AO16" s="75"/>
+      <c r="AP16" s="75"/>
+      <c r="AQ16" s="75"/>
+      <c r="AR16" s="75"/>
+      <c r="AS16" s="75"/>
+      <c r="AT16" s="75"/>
+      <c r="AU16" s="75"/>
       <c r="AV16" s="38"/>
       <c r="AW16" s="38"/>
       <c r="AX16" s="38"/>
@@ -2976,52 +2979,52 @@
       </c>
       <c r="C17" s="63"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="88"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I17" s="38"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
-      <c r="S17" s="81"/>
-      <c r="T17" s="81"/>
-      <c r="U17" s="81"/>
-      <c r="V17" s="81"/>
-      <c r="W17" s="81"/>
-      <c r="X17" s="81"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="81"/>
-      <c r="AA17" s="81"/>
-      <c r="AB17" s="81"/>
-      <c r="AC17" s="81"/>
-      <c r="AD17" s="81"/>
-      <c r="AE17" s="81"/>
-      <c r="AF17" s="81"/>
-      <c r="AG17" s="81"/>
-      <c r="AH17" s="81"/>
-      <c r="AI17" s="81"/>
-      <c r="AJ17" s="81"/>
-      <c r="AK17" s="81"/>
-      <c r="AL17" s="81"/>
-      <c r="AM17" s="81"/>
-      <c r="AN17" s="81"/>
-      <c r="AO17" s="81"/>
-      <c r="AP17" s="81"/>
-      <c r="AQ17" s="81"/>
-      <c r="AR17" s="81"/>
-      <c r="AS17" s="81"/>
-      <c r="AT17" s="81"/>
-      <c r="AU17" s="81"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="75"/>
+      <c r="V17" s="75"/>
+      <c r="W17" s="75"/>
+      <c r="X17" s="75"/>
+      <c r="Y17" s="75"/>
+      <c r="Z17" s="75"/>
+      <c r="AA17" s="75"/>
+      <c r="AB17" s="75"/>
+      <c r="AC17" s="75"/>
+      <c r="AD17" s="75"/>
+      <c r="AE17" s="75"/>
+      <c r="AF17" s="75"/>
+      <c r="AG17" s="75"/>
+      <c r="AH17" s="75"/>
+      <c r="AI17" s="75"/>
+      <c r="AJ17" s="75"/>
+      <c r="AK17" s="75"/>
+      <c r="AL17" s="75"/>
+      <c r="AM17" s="75"/>
+      <c r="AN17" s="75"/>
+      <c r="AO17" s="75"/>
+      <c r="AP17" s="75"/>
+      <c r="AQ17" s="75"/>
+      <c r="AR17" s="75"/>
+      <c r="AS17" s="75"/>
+      <c r="AT17" s="75"/>
+      <c r="AU17" s="75"/>
       <c r="AV17" s="38"/>
       <c r="AW17" s="38"/>
       <c r="AX17" s="38"/>
@@ -3042,20 +3045,20 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="51"/>
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="90" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="28">
         <v>1</v>
       </c>
-      <c r="E18" s="89">
+      <c r="E18" s="83">
         <f>F11+0</f>
         <v>44642</v>
       </c>
-      <c r="F18" s="89">
+      <c r="F18" s="83">
         <f>E18+0</f>
         <v>44642</v>
       </c>
@@ -3065,44 +3068,44 @@
         <v>1</v>
       </c>
       <c r="I18" s="38"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="81"/>
-      <c r="S18" s="81"/>
-      <c r="T18" s="81"/>
-      <c r="U18" s="81"/>
-      <c r="V18" s="81"/>
-      <c r="W18" s="81"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="81"/>
-      <c r="Z18" s="81"/>
-      <c r="AA18" s="81"/>
-      <c r="AB18" s="81"/>
-      <c r="AC18" s="81"/>
-      <c r="AD18" s="81"/>
-      <c r="AE18" s="81"/>
-      <c r="AF18" s="81"/>
-      <c r="AG18" s="81"/>
-      <c r="AH18" s="81"/>
-      <c r="AI18" s="81"/>
-      <c r="AJ18" s="81"/>
-      <c r="AK18" s="81"/>
-      <c r="AL18" s="81"/>
-      <c r="AM18" s="81"/>
-      <c r="AN18" s="81"/>
-      <c r="AO18" s="81"/>
-      <c r="AP18" s="81"/>
-      <c r="AQ18" s="81"/>
-      <c r="AR18" s="81"/>
-      <c r="AS18" s="81"/>
-      <c r="AT18" s="81"/>
-      <c r="AU18" s="81"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="75"/>
+      <c r="U18" s="75"/>
+      <c r="V18" s="75"/>
+      <c r="W18" s="75"/>
+      <c r="X18" s="75"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="75"/>
+      <c r="AA18" s="75"/>
+      <c r="AB18" s="75"/>
+      <c r="AC18" s="75"/>
+      <c r="AD18" s="75"/>
+      <c r="AE18" s="75"/>
+      <c r="AF18" s="75"/>
+      <c r="AG18" s="75"/>
+      <c r="AH18" s="75"/>
+      <c r="AI18" s="75"/>
+      <c r="AJ18" s="75"/>
+      <c r="AK18" s="75"/>
+      <c r="AL18" s="75"/>
+      <c r="AM18" s="75"/>
+      <c r="AN18" s="75"/>
+      <c r="AO18" s="75"/>
+      <c r="AP18" s="75"/>
+      <c r="AQ18" s="75"/>
+      <c r="AR18" s="75"/>
+      <c r="AS18" s="75"/>
+      <c r="AT18" s="75"/>
+      <c r="AU18" s="75"/>
       <c r="AV18" s="38"/>
       <c r="AW18" s="38"/>
       <c r="AX18" s="38"/>
@@ -3123,20 +3126,20 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="51"/>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="90" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="28">
         <v>1</v>
       </c>
-      <c r="E19" s="89">
+      <c r="E19" s="83">
         <f>F18+0</f>
         <v>44642</v>
       </c>
-      <c r="F19" s="89">
+      <c r="F19" s="83">
         <f>E19+1</f>
         <v>44643</v>
       </c>
@@ -3146,44 +3149,44 @@
         <v>2</v>
       </c>
       <c r="I19" s="38"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
-      <c r="S19" s="81"/>
-      <c r="T19" s="81"/>
-      <c r="U19" s="81"/>
-      <c r="V19" s="81"/>
-      <c r="W19" s="81"/>
-      <c r="X19" s="81"/>
-      <c r="Y19" s="81"/>
-      <c r="Z19" s="81"/>
-      <c r="AA19" s="81"/>
-      <c r="AB19" s="81"/>
-      <c r="AC19" s="81"/>
-      <c r="AD19" s="81"/>
-      <c r="AE19" s="81"/>
-      <c r="AF19" s="81"/>
-      <c r="AG19" s="81"/>
-      <c r="AH19" s="81"/>
-      <c r="AI19" s="81"/>
-      <c r="AJ19" s="81"/>
-      <c r="AK19" s="81"/>
-      <c r="AL19" s="81"/>
-      <c r="AM19" s="81"/>
-      <c r="AN19" s="81"/>
-      <c r="AO19" s="81"/>
-      <c r="AP19" s="81"/>
-      <c r="AQ19" s="81"/>
-      <c r="AR19" s="81"/>
-      <c r="AS19" s="81"/>
-      <c r="AT19" s="81"/>
-      <c r="AU19" s="81"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="75"/>
+      <c r="V19" s="75"/>
+      <c r="W19" s="75"/>
+      <c r="X19" s="75"/>
+      <c r="Y19" s="75"/>
+      <c r="Z19" s="75"/>
+      <c r="AA19" s="75"/>
+      <c r="AB19" s="75"/>
+      <c r="AC19" s="75"/>
+      <c r="AD19" s="75"/>
+      <c r="AE19" s="75"/>
+      <c r="AF19" s="75"/>
+      <c r="AG19" s="75"/>
+      <c r="AH19" s="75"/>
+      <c r="AI19" s="75"/>
+      <c r="AJ19" s="75"/>
+      <c r="AK19" s="75"/>
+      <c r="AL19" s="75"/>
+      <c r="AM19" s="75"/>
+      <c r="AN19" s="75"/>
+      <c r="AO19" s="75"/>
+      <c r="AP19" s="75"/>
+      <c r="AQ19" s="75"/>
+      <c r="AR19" s="75"/>
+      <c r="AS19" s="75"/>
+      <c r="AT19" s="75"/>
+      <c r="AU19" s="75"/>
       <c r="AV19" s="38"/>
       <c r="AW19" s="38"/>
       <c r="AX19" s="38"/>
@@ -3204,20 +3207,20 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="51"/>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="90" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="28">
         <v>1</v>
       </c>
-      <c r="E20" s="89">
+      <c r="E20" s="83">
         <f>F19+0</f>
         <v>44643</v>
       </c>
-      <c r="F20" s="89">
+      <c r="F20" s="83">
         <f>E20+0</f>
         <v>44643</v>
       </c>
@@ -3227,44 +3230,44 @@
         <v>1</v>
       </c>
       <c r="I20" s="38"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="81"/>
-      <c r="S20" s="81"/>
-      <c r="T20" s="81"/>
-      <c r="U20" s="81"/>
-      <c r="V20" s="81"/>
-      <c r="W20" s="81"/>
-      <c r="X20" s="81"/>
-      <c r="Y20" s="81"/>
-      <c r="Z20" s="81"/>
-      <c r="AA20" s="81"/>
-      <c r="AB20" s="81"/>
-      <c r="AC20" s="81"/>
-      <c r="AD20" s="81"/>
-      <c r="AE20" s="81"/>
-      <c r="AF20" s="81"/>
-      <c r="AG20" s="81"/>
-      <c r="AH20" s="81"/>
-      <c r="AI20" s="81"/>
-      <c r="AJ20" s="81"/>
-      <c r="AK20" s="81"/>
-      <c r="AL20" s="81"/>
-      <c r="AM20" s="81"/>
-      <c r="AN20" s="81"/>
-      <c r="AO20" s="81"/>
-      <c r="AP20" s="81"/>
-      <c r="AQ20" s="81"/>
-      <c r="AR20" s="81"/>
-      <c r="AS20" s="81"/>
-      <c r="AT20" s="81"/>
-      <c r="AU20" s="81"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="75"/>
+      <c r="W20" s="75"/>
+      <c r="X20" s="75"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="75"/>
+      <c r="AA20" s="75"/>
+      <c r="AB20" s="75"/>
+      <c r="AC20" s="75"/>
+      <c r="AD20" s="75"/>
+      <c r="AE20" s="75"/>
+      <c r="AF20" s="75"/>
+      <c r="AG20" s="75"/>
+      <c r="AH20" s="75"/>
+      <c r="AI20" s="75"/>
+      <c r="AJ20" s="75"/>
+      <c r="AK20" s="75"/>
+      <c r="AL20" s="75"/>
+      <c r="AM20" s="75"/>
+      <c r="AN20" s="75"/>
+      <c r="AO20" s="75"/>
+      <c r="AP20" s="75"/>
+      <c r="AQ20" s="75"/>
+      <c r="AR20" s="75"/>
+      <c r="AS20" s="75"/>
+      <c r="AT20" s="75"/>
+      <c r="AU20" s="75"/>
       <c r="AV20" s="38"/>
       <c r="AW20" s="38"/>
       <c r="AX20" s="38"/>
@@ -3285,64 +3288,64 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="51"/>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="90" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="28">
         <v>1</v>
       </c>
-      <c r="E21" s="89">
+      <c r="E21" s="83">
         <f>F20+1</f>
         <v>44644</v>
       </c>
-      <c r="F21" s="89">
+      <c r="F21" s="83">
         <f>E21+0</f>
         <v>44644</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="38"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
-      <c r="S21" s="81"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="81"/>
-      <c r="V21" s="81"/>
-      <c r="W21" s="81"/>
-      <c r="X21" s="81"/>
-      <c r="Y21" s="81"/>
-      <c r="Z21" s="81"/>
-      <c r="AA21" s="81"/>
-      <c r="AB21" s="81"/>
-      <c r="AC21" s="81"/>
-      <c r="AD21" s="81"/>
-      <c r="AE21" s="81"/>
-      <c r="AF21" s="81"/>
-      <c r="AG21" s="81"/>
-      <c r="AH21" s="81"/>
-      <c r="AI21" s="81"/>
-      <c r="AJ21" s="81"/>
-      <c r="AK21" s="81"/>
-      <c r="AL21" s="81"/>
-      <c r="AM21" s="81"/>
-      <c r="AN21" s="81"/>
-      <c r="AO21" s="81"/>
-      <c r="AP21" s="81"/>
-      <c r="AQ21" s="81"/>
-      <c r="AR21" s="81"/>
-      <c r="AS21" s="81"/>
-      <c r="AT21" s="81"/>
-      <c r="AU21" s="81"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="75"/>
+      <c r="X21" s="75"/>
+      <c r="Y21" s="75"/>
+      <c r="Z21" s="75"/>
+      <c r="AA21" s="75"/>
+      <c r="AB21" s="75"/>
+      <c r="AC21" s="75"/>
+      <c r="AD21" s="75"/>
+      <c r="AE21" s="75"/>
+      <c r="AF21" s="75"/>
+      <c r="AG21" s="75"/>
+      <c r="AH21" s="75"/>
+      <c r="AI21" s="75"/>
+      <c r="AJ21" s="75"/>
+      <c r="AK21" s="75"/>
+      <c r="AL21" s="75"/>
+      <c r="AM21" s="75"/>
+      <c r="AN21" s="75"/>
+      <c r="AO21" s="75"/>
+      <c r="AP21" s="75"/>
+      <c r="AQ21" s="75"/>
+      <c r="AR21" s="75"/>
+      <c r="AS21" s="75"/>
+      <c r="AT21" s="75"/>
+      <c r="AU21" s="75"/>
       <c r="AV21" s="38"/>
       <c r="AW21" s="38"/>
       <c r="AX21" s="38"/>
@@ -3363,64 +3366,64 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="51"/>
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="96" t="s">
+      <c r="C22" s="90" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="28">
         <v>1</v>
       </c>
-      <c r="E22" s="89">
+      <c r="E22" s="83">
         <f>F21+0</f>
         <v>44644</v>
       </c>
-      <c r="F22" s="89">
+      <c r="F22" s="83">
         <f>E22+1</f>
         <v>44645</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="38"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="81"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="81"/>
-      <c r="V22" s="81"/>
-      <c r="W22" s="81"/>
-      <c r="X22" s="81"/>
-      <c r="Y22" s="81"/>
-      <c r="Z22" s="81"/>
-      <c r="AA22" s="81"/>
-      <c r="AB22" s="81"/>
-      <c r="AC22" s="81"/>
-      <c r="AD22" s="81"/>
-      <c r="AE22" s="81"/>
-      <c r="AF22" s="81"/>
-      <c r="AG22" s="81"/>
-      <c r="AH22" s="81"/>
-      <c r="AI22" s="81"/>
-      <c r="AJ22" s="81"/>
-      <c r="AK22" s="81"/>
-      <c r="AL22" s="81"/>
-      <c r="AM22" s="81"/>
-      <c r="AN22" s="81"/>
-      <c r="AO22" s="81"/>
-      <c r="AP22" s="81"/>
-      <c r="AQ22" s="81"/>
-      <c r="AR22" s="81"/>
-      <c r="AS22" s="81"/>
-      <c r="AT22" s="81"/>
-      <c r="AU22" s="81"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="75"/>
+      <c r="V22" s="75"/>
+      <c r="W22" s="75"/>
+      <c r="X22" s="75"/>
+      <c r="Y22" s="75"/>
+      <c r="Z22" s="75"/>
+      <c r="AA22" s="75"/>
+      <c r="AB22" s="75"/>
+      <c r="AC22" s="75"/>
+      <c r="AD22" s="75"/>
+      <c r="AE22" s="75"/>
+      <c r="AF22" s="75"/>
+      <c r="AG22" s="75"/>
+      <c r="AH22" s="75"/>
+      <c r="AI22" s="75"/>
+      <c r="AJ22" s="75"/>
+      <c r="AK22" s="75"/>
+      <c r="AL22" s="75"/>
+      <c r="AM22" s="75"/>
+      <c r="AN22" s="75"/>
+      <c r="AO22" s="75"/>
+      <c r="AP22" s="75"/>
+      <c r="AQ22" s="75"/>
+      <c r="AR22" s="75"/>
+      <c r="AS22" s="75"/>
+      <c r="AT22" s="75"/>
+      <c r="AU22" s="75"/>
       <c r="AV22" s="38"/>
       <c r="AW22" s="38"/>
       <c r="AX22" s="38"/>
@@ -3440,60 +3443,65 @@
       <c r="BL22" s="38"/>
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="91"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="90" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="28">
+        <v>1</v>
+      </c>
+      <c r="E23" s="83">
+        <f>F22+3</f>
+        <v>44648</v>
+      </c>
+      <c r="F23" s="83">
+        <f>E23+3</f>
+        <v>44651</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H23" s="17"/>
       <c r="I23" s="38"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="81"/>
-      <c r="O23" s="81"/>
-      <c r="P23" s="81"/>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="81"/>
-      <c r="S23" s="81"/>
-      <c r="T23" s="81"/>
-      <c r="U23" s="81"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
-      <c r="X23" s="81"/>
-      <c r="Y23" s="81"/>
-      <c r="Z23" s="81"/>
-      <c r="AA23" s="81"/>
-      <c r="AB23" s="81"/>
-      <c r="AC23" s="81"/>
-      <c r="AD23" s="81"/>
-      <c r="AE23" s="81"/>
-      <c r="AF23" s="81"/>
-      <c r="AG23" s="81"/>
-      <c r="AH23" s="81"/>
-      <c r="AI23" s="81"/>
-      <c r="AJ23" s="81"/>
-      <c r="AK23" s="81"/>
-      <c r="AL23" s="81"/>
-      <c r="AM23" s="81"/>
-      <c r="AN23" s="81"/>
-      <c r="AO23" s="81"/>
-      <c r="AP23" s="81"/>
-      <c r="AQ23" s="81"/>
-      <c r="AR23" s="81"/>
-      <c r="AS23" s="81"/>
-      <c r="AT23" s="81"/>
-      <c r="AU23" s="81"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="75"/>
+      <c r="V23" s="75"/>
+      <c r="W23" s="75"/>
+      <c r="X23" s="75"/>
+      <c r="Y23" s="75"/>
+      <c r="Z23" s="75"/>
+      <c r="AA23" s="75"/>
+      <c r="AB23" s="75"/>
+      <c r="AC23" s="75"/>
+      <c r="AD23" s="75"/>
+      <c r="AE23" s="75"/>
+      <c r="AF23" s="75"/>
+      <c r="AG23" s="75"/>
+      <c r="AH23" s="75"/>
+      <c r="AI23" s="75"/>
+      <c r="AJ23" s="75"/>
+      <c r="AK23" s="75"/>
+      <c r="AL23" s="75"/>
+      <c r="AM23" s="75"/>
+      <c r="AN23" s="75"/>
+      <c r="AO23" s="75"/>
+      <c r="AP23" s="75"/>
+      <c r="AQ23" s="75"/>
+      <c r="AR23" s="75"/>
+      <c r="AS23" s="75"/>
+      <c r="AT23" s="75"/>
+      <c r="AU23" s="75"/>
       <c r="AV23" s="38"/>
       <c r="AW23" s="38"/>
       <c r="AX23" s="38"/>
@@ -3513,62 +3521,60 @@
       <c r="BL23" s="38"/>
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="51"/>
-      <c r="B24" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="92" t="s">
-        <v>27</v>
-      </c>
+      <c r="A24" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="17" t="e">
+      <c r="H24" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="38"/>
-      <c r="AC24" s="38"/>
-      <c r="AD24" s="38"/>
-      <c r="AE24" s="38"/>
-      <c r="AF24" s="38"/>
-      <c r="AG24" s="38"/>
-      <c r="AH24" s="38"/>
-      <c r="AI24" s="38"/>
-      <c r="AJ24" s="38"/>
-      <c r="AK24" s="38"/>
-      <c r="AL24" s="38"/>
-      <c r="AM24" s="38"/>
-      <c r="AN24" s="38"/>
-      <c r="AO24" s="38"/>
-      <c r="AP24" s="38"/>
-      <c r="AQ24" s="38"/>
-      <c r="AR24" s="38"/>
-      <c r="AS24" s="38"/>
-      <c r="AT24" s="38"/>
-      <c r="AU24" s="38"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="75"/>
+      <c r="T24" s="75"/>
+      <c r="U24" s="75"/>
+      <c r="V24" s="75"/>
+      <c r="W24" s="75"/>
+      <c r="X24" s="75"/>
+      <c r="Y24" s="75"/>
+      <c r="Z24" s="75"/>
+      <c r="AA24" s="75"/>
+      <c r="AB24" s="75"/>
+      <c r="AC24" s="75"/>
+      <c r="AD24" s="75"/>
+      <c r="AE24" s="75"/>
+      <c r="AF24" s="75"/>
+      <c r="AG24" s="75"/>
+      <c r="AH24" s="75"/>
+      <c r="AI24" s="75"/>
+      <c r="AJ24" s="75"/>
+      <c r="AK24" s="75"/>
+      <c r="AL24" s="75"/>
+      <c r="AM24" s="75"/>
+      <c r="AN24" s="75"/>
+      <c r="AO24" s="75"/>
+      <c r="AP24" s="75"/>
+      <c r="AQ24" s="75"/>
+      <c r="AR24" s="75"/>
+      <c r="AS24" s="75"/>
+      <c r="AT24" s="75"/>
+      <c r="AU24" s="75"/>
       <c r="AV24" s="38"/>
       <c r="AW24" s="38"/>
       <c r="AX24" s="38"/>
@@ -3589,15 +3595,15 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="51"/>
-      <c r="B25" s="95" t="s">
-        <v>61</v>
+      <c r="B25" s="89" t="s">
+        <v>60</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="31"/>
-      <c r="E25" s="92" t="s">
+      <c r="E25" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="92" t="s">
+      <c r="F25" s="86" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="17"/>
@@ -3664,15 +3670,15 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="51"/>
-      <c r="B26" s="69" t="s">
-        <v>0</v>
+      <c r="B26" s="89" t="s">
+        <v>61</v>
       </c>
       <c r="C26" s="65"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="92" t="s">
+      <c r="E26" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="92" t="s">
+      <c r="F26" s="86" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="17"/>
@@ -3740,14 +3746,14 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="51"/>
       <c r="B27" s="69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="31"/>
-      <c r="E27" s="92" t="s">
+      <c r="E27" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="92" t="s">
+      <c r="F27" s="86" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="17"/>
@@ -3815,14 +3821,14 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="51"/>
       <c r="B28" s="69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="31"/>
-      <c r="E28" s="92" t="s">
+      <c r="E28" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="92" t="s">
+      <c r="F28" s="86" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="17"/>
@@ -3888,18 +3894,22 @@
       <c r="BL28" s="38"/>
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="65"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="86" t="s">
+        <v>27</v>
+      </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="17" t="str">
+      <c r="H29" s="17" t="e">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I29" s="38"/>
       <c r="J29" s="38"/>
@@ -3959,96 +3969,167 @@
       <c r="BL29" s="38"/>
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="52"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="39"/>
-      <c r="T30" s="39"/>
-      <c r="U30" s="39"/>
-      <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
-      <c r="X30" s="39"/>
-      <c r="Y30" s="39"/>
-      <c r="Z30" s="39"/>
-      <c r="AA30" s="39"/>
-      <c r="AB30" s="39"/>
-      <c r="AC30" s="39"/>
-      <c r="AD30" s="39"/>
-      <c r="AE30" s="39"/>
-      <c r="AF30" s="39"/>
-      <c r="AG30" s="39"/>
-      <c r="AH30" s="39"/>
-      <c r="AI30" s="39"/>
-      <c r="AJ30" s="39"/>
-      <c r="AK30" s="39"/>
-      <c r="AL30" s="39"/>
-      <c r="AM30" s="39"/>
-      <c r="AN30" s="39"/>
-      <c r="AO30" s="39"/>
-      <c r="AP30" s="39"/>
-      <c r="AQ30" s="39"/>
-      <c r="AR30" s="39"/>
-      <c r="AS30" s="39"/>
-      <c r="AT30" s="39"/>
-      <c r="AU30" s="39"/>
-      <c r="AV30" s="39"/>
-      <c r="AW30" s="39"/>
-      <c r="AX30" s="39"/>
-      <c r="AY30" s="39"/>
-      <c r="AZ30" s="39"/>
-      <c r="BA30" s="39"/>
-      <c r="BB30" s="39"/>
-      <c r="BC30" s="39"/>
-      <c r="BD30" s="39"/>
-      <c r="BE30" s="39"/>
-      <c r="BF30" s="39"/>
-      <c r="BG30" s="39"/>
-      <c r="BH30" s="39"/>
-      <c r="BI30" s="39"/>
-      <c r="BJ30" s="39"/>
-      <c r="BK30" s="39"/>
-      <c r="BL30" s="39"/>
-    </row>
-    <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="6"/>
+      <c r="A30" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="70"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="38"/>
+      <c r="X30" s="38"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="38"/>
+      <c r="AB30" s="38"/>
+      <c r="AC30" s="38"/>
+      <c r="AD30" s="38"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="38"/>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="38"/>
+      <c r="AI30" s="38"/>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="38"/>
+      <c r="AL30" s="38"/>
+      <c r="AM30" s="38"/>
+      <c r="AN30" s="38"/>
+      <c r="AO30" s="38"/>
+      <c r="AP30" s="38"/>
+      <c r="AQ30" s="38"/>
+      <c r="AR30" s="38"/>
+      <c r="AS30" s="38"/>
+      <c r="AT30" s="38"/>
+      <c r="AU30" s="38"/>
+      <c r="AV30" s="38"/>
+      <c r="AW30" s="38"/>
+      <c r="AX30" s="38"/>
+      <c r="AY30" s="38"/>
+      <c r="AZ30" s="38"/>
+      <c r="BA30" s="38"/>
+      <c r="BB30" s="38"/>
+      <c r="BC30" s="38"/>
+      <c r="BD30" s="38"/>
+      <c r="BE30" s="38"/>
+      <c r="BF30" s="38"/>
+      <c r="BG30" s="38"/>
+      <c r="BH30" s="38"/>
+      <c r="BI30" s="38"/>
+      <c r="BJ30" s="38"/>
+      <c r="BK30" s="38"/>
+      <c r="BL30" s="38"/>
+    </row>
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="52"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="39"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="39"/>
+      <c r="AB31" s="39"/>
+      <c r="AC31" s="39"/>
+      <c r="AD31" s="39"/>
+      <c r="AE31" s="39"/>
+      <c r="AF31" s="39"/>
+      <c r="AG31" s="39"/>
+      <c r="AH31" s="39"/>
+      <c r="AI31" s="39"/>
+      <c r="AJ31" s="39"/>
+      <c r="AK31" s="39"/>
+      <c r="AL31" s="39"/>
+      <c r="AM31" s="39"/>
+      <c r="AN31" s="39"/>
+      <c r="AO31" s="39"/>
+      <c r="AP31" s="39"/>
+      <c r="AQ31" s="39"/>
+      <c r="AR31" s="39"/>
+      <c r="AS31" s="39"/>
+      <c r="AT31" s="39"/>
+      <c r="AU31" s="39"/>
+      <c r="AV31" s="39"/>
+      <c r="AW31" s="39"/>
+      <c r="AX31" s="39"/>
+      <c r="AY31" s="39"/>
+      <c r="AZ31" s="39"/>
+      <c r="BA31" s="39"/>
+      <c r="BB31" s="39"/>
+      <c r="BC31" s="39"/>
+      <c r="BD31" s="39"/>
+      <c r="BE31" s="39"/>
+      <c r="BF31" s="39"/>
+      <c r="BG31" s="39"/>
+      <c r="BH31" s="39"/>
+      <c r="BI31" s="39"/>
+      <c r="BJ31" s="39"/>
+      <c r="BK31" s="39"/>
+      <c r="BL31" s="39"/>
     </row>
     <row r="32" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="14"/>
-      <c r="F32" s="53"/>
-    </row>
-    <row r="33" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="15"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="14"/>
+      <c r="F33" s="53"/>
+    </row>
+    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D30">
+  <conditionalFormatting sqref="D7:D31">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4062,12 +4143,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL30">
+  <conditionalFormatting sqref="I5:BL31">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL30">
+  <conditionalFormatting sqref="I7:BL31">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4102,7 +4183,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D30</xm:sqref>
+          <xm:sqref>D7:D31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>